<commit_message>
feat - loginview View ViewModel 분리           View 코드 줄이기 - customView 구현(textfield 부분)
</commit_message>
<xml_diff>
--- a/복사본 STUDYHUB QA.xlsx
+++ b/복사본 STUDYHUB QA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yong/Desktop/study-hub-iOS-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A343063-0462-AE4D-92A4-5BE31C88AC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15C93DE-3508-8A43-94EB-CE18D0680AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19440" yWindow="1080" windowWidth="23820" windowHeight="26840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
@@ -1067,9 +1067,6 @@
     <t>비밀번호가 일치하지 않으면 '다음' 버튼 비활성화, 모든 항목이 일치한다는 코멘트가 뜰 경우에만 활성화 버튼으로 변경</t>
   </si>
   <si>
-    <t>비회원-스터디 상세</t>
-  </si>
-  <si>
     <t>텍스트 필드를 누르면 바로 로그인 팝업이 뜨도록 수정 필요</t>
   </si>
   <si>
@@ -1097,9 +1094,6 @@
     <t>모든 행동</t>
   </si>
   <si>
-    <t>모든 버튼을 두번누르면 두번들어감 (작성 두번누르면 두번 작성됨)</t>
-  </si>
-  <si>
     <t>_x0008_작동중이라면 뺑글뻉글 돌아가는게 보여야지 두번누를일이 없을듯 합니다 ㅠ</t>
   </si>
   <si>
@@ -1142,19 +1136,7 @@
     <t>기간 외에 다른 것만 수정해도 '완료하기'버튼을 누를 수 있도록 수정 필요</t>
   </si>
   <si>
-    <t>스터디 / 스터디 상세</t>
-  </si>
-  <si>
-    <t>인원 수 수정 후, 스터디 탭에서는 인원 수가 갑자기 절반 이상 채워짐 / 스터디 상세로 들어가면 수정 이전 인원 수가 그대로임</t>
-  </si>
-  <si>
     <t>스터디 수정 인원 수가 스터디 탭, 스터디 상세 페이지 모두 제대로 반영되도록 수정 필요</t>
-  </si>
-  <si>
-    <t>_x0008_스터디 수락 후 참여자 목록</t>
-  </si>
-  <si>
-    <t>_x0008_수락한것들 참여자 들어가면 아무것도 안보임</t>
   </si>
   <si>
     <t>_x0008__x0008_착성한 글 리스트</t>
@@ -1946,6 +1928,619 @@
       </rPr>
       <t>)</t>
     </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>비회원-스터디 상세</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>_x0008_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>스터디</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>수락</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>후</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>참여자</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>목록</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>_x0008_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>수락한것들</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>참여자</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>들어가면</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>아무것도</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>안보임</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>스터디</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>스터디</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>상세</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>인원</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>수</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>수정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>후</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>스터디</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>탭에서는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>인원</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>수가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>갑자기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>절반</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>이상</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>채워짐</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>스터디</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>상세로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>들어가면</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>수정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>이전</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>인원</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>수가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+      </rPr>
+      <t>그대로임</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 버튼을 두번누르면 두번들어감 (작성 두번누르면 두번 작성됨)</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -2065,7 +2660,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2150,6 +2745,18 @@
         <bgColor rgb="FFFCE5CD"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -2213,7 +2820,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2338,6 +2945,18 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2574,8 +3193,8 @@
   </sheetPr>
   <dimension ref="A1:P196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="D145" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G159" sqref="G159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2593,27 +3212,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1" s="52" t="s">
-        <v>401</v>
-      </c>
-      <c r="B1" s="51"/>
+      <c r="A1" s="56" t="s">
+        <v>395</v>
+      </c>
+      <c r="B1" s="55"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="51"/>
-      <c r="G1" s="53" t="s">
+      <c r="F1" s="55"/>
+      <c r="G1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
       <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2627,8 +3246,8 @@
     </row>
     <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="4"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="51"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="55"/>
       <c r="M3" s="6" t="s">
         <v>6</v>
       </c>
@@ -2658,27 +3277,27 @@
       <c r="M5" s="2"/>
     </row>
     <row r="6" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="51"/>
+      <c r="B6" s="55"/>
     </row>
     <row r="7" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2698,21 +3317,21 @@
       <c r="M10" s="2"/>
     </row>
     <row r="11" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
       <c r="M11" s="2"/>
     </row>
     <row r="12" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A12" s="50" t="s">
+      <c r="A12" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
       <c r="M12" s="2"/>
     </row>
     <row r="13" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -4341,7 +4960,7 @@
         <v>31</v>
       </c>
       <c r="G72" s="43" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="H72" s="19" t="s">
         <v>159</v>
@@ -4969,7 +5588,7 @@
       </c>
       <c r="I94" s="2"/>
     </row>
-    <row r="95" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="2" t="s">
         <v>216</v>
       </c>
@@ -4980,7 +5599,7 @@
         <v>21</v>
       </c>
       <c r="D95" s="44" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>217</v>
@@ -5002,7 +5621,7 @@
       <c r="L95" s="2"/>
       <c r="M95" s="2"/>
     </row>
-    <row r="96" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="2" t="s">
         <v>216</v>
       </c>
@@ -5013,7 +5632,7 @@
         <v>21</v>
       </c>
       <c r="D96" s="44" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>222</v>
@@ -5037,7 +5656,7 @@
       </c>
       <c r="M96" s="2"/>
     </row>
-    <row r="97" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A97" s="40" t="s">
         <v>26</v>
       </c>
@@ -5048,7 +5667,7 @@
         <v>21</v>
       </c>
       <c r="D97" s="45" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E97" s="40" t="s">
         <v>217</v>
@@ -5070,7 +5689,7 @@
       <c r="L97" s="41"/>
       <c r="M97" s="2"/>
     </row>
-    <row r="98" spans="1:13" ht="14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:13" ht="14" x14ac:dyDescent="0.15">
       <c r="A98" s="2" t="s">
         <v>26</v>
       </c>
@@ -5081,7 +5700,7 @@
         <v>21</v>
       </c>
       <c r="D98" s="46" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>217</v>
@@ -5103,7 +5722,7 @@
       <c r="L98" s="2"/>
       <c r="M98" s="2"/>
     </row>
-    <row r="99" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A99" s="2" t="s">
         <v>26</v>
       </c>
@@ -5114,7 +5733,7 @@
         <v>21</v>
       </c>
       <c r="D99" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>64</v>
@@ -5136,7 +5755,7 @@
       <c r="L99" s="2"/>
       <c r="M99" s="2"/>
     </row>
-    <row r="100" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A100" s="2" t="s">
         <v>26</v>
       </c>
@@ -5147,7 +5766,7 @@
         <v>21</v>
       </c>
       <c r="D100" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>232</v>
@@ -5169,7 +5788,7 @@
       <c r="L100" s="2"/>
       <c r="M100" s="2"/>
     </row>
-    <row r="101" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A101" s="2" t="s">
         <v>26</v>
       </c>
@@ -5180,7 +5799,7 @@
         <v>21</v>
       </c>
       <c r="D101" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>235</v>
@@ -5202,7 +5821,7 @@
       <c r="L101" s="2"/>
       <c r="M101" s="2"/>
     </row>
-    <row r="102" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A102" s="2" t="s">
         <v>26</v>
       </c>
@@ -5213,7 +5832,7 @@
         <v>21</v>
       </c>
       <c r="D102" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>238</v>
@@ -5235,7 +5854,7 @@
       <c r="L102" s="2"/>
       <c r="M102" s="2"/>
     </row>
-    <row r="103" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A103" s="2" t="s">
         <v>26</v>
       </c>
@@ -5246,7 +5865,7 @@
         <v>21</v>
       </c>
       <c r="D103" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>241</v>
@@ -5268,7 +5887,7 @@
       <c r="L103" s="2"/>
       <c r="M103" s="2"/>
     </row>
-    <row r="104" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A104" s="2" t="s">
         <v>26</v>
       </c>
@@ -5279,7 +5898,7 @@
         <v>21</v>
       </c>
       <c r="D104" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>244</v>
@@ -5301,7 +5920,7 @@
       <c r="L104" s="2"/>
       <c r="M104" s="2"/>
     </row>
-    <row r="105" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A105" s="2" t="s">
         <v>26</v>
       </c>
@@ -5312,7 +5931,7 @@
         <v>21</v>
       </c>
       <c r="D105" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>247</v>
@@ -5334,7 +5953,7 @@
       <c r="L105" s="2"/>
       <c r="M105" s="2"/>
     </row>
-    <row r="106" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A106" s="2" t="s">
         <v>26</v>
       </c>
@@ -5345,7 +5964,7 @@
         <v>21</v>
       </c>
       <c r="D106" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>250</v>
@@ -5367,7 +5986,7 @@
       <c r="L106" s="2"/>
       <c r="M106" s="2"/>
     </row>
-    <row r="107" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A107" s="2" t="s">
         <v>26</v>
       </c>
@@ -5378,7 +5997,7 @@
         <v>21</v>
       </c>
       <c r="D107" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>64</v>
@@ -5400,7 +6019,7 @@
       <c r="L107" s="2"/>
       <c r="M107" s="2"/>
     </row>
-    <row r="108" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A108" s="2" t="s">
         <v>26</v>
       </c>
@@ -5411,7 +6030,7 @@
         <v>21</v>
       </c>
       <c r="D108" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>255</v>
@@ -5433,7 +6052,7 @@
       <c r="L108" s="2"/>
       <c r="M108" s="2"/>
     </row>
-    <row r="109" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A109" s="2" t="s">
         <v>26</v>
       </c>
@@ -5444,7 +6063,7 @@
         <v>21</v>
       </c>
       <c r="D109" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>255</v>
@@ -5466,7 +6085,7 @@
       <c r="L109" s="2"/>
       <c r="M109" s="2"/>
     </row>
-    <row r="110" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A110" s="2" t="s">
         <v>26</v>
       </c>
@@ -5477,7 +6096,7 @@
         <v>21</v>
       </c>
       <c r="D110" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>255</v>
@@ -5499,7 +6118,7 @@
       <c r="L110" s="2"/>
       <c r="M110" s="2"/>
     </row>
-    <row r="111" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A111" s="2" t="s">
         <v>26</v>
       </c>
@@ -5510,7 +6129,7 @@
         <v>21</v>
       </c>
       <c r="D111" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>30</v>
@@ -5532,7 +6151,7 @@
       <c r="L111" s="2"/>
       <c r="M111" s="2"/>
     </row>
-    <row r="112" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A112" s="2" t="s">
         <v>26</v>
       </c>
@@ -5543,7 +6162,7 @@
         <v>21</v>
       </c>
       <c r="D112" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>30</v>
@@ -5565,7 +6184,7 @@
       <c r="L112" s="2"/>
       <c r="M112" s="2"/>
     </row>
-    <row r="113" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A113" s="2" t="s">
         <v>26</v>
       </c>
@@ -5576,7 +6195,7 @@
         <v>21</v>
       </c>
       <c r="D113" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>30</v>
@@ -5598,7 +6217,7 @@
       <c r="L113" s="2"/>
       <c r="M113" s="2"/>
     </row>
-    <row r="114" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A114" s="2" t="s">
         <v>26</v>
       </c>
@@ -5609,7 +6228,7 @@
         <v>21</v>
       </c>
       <c r="D114" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>268</v>
@@ -5631,7 +6250,7 @@
       <c r="L114" s="2"/>
       <c r="M114" s="2"/>
     </row>
-    <row r="115" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A115" s="2" t="s">
         <v>26</v>
       </c>
@@ -5642,7 +6261,7 @@
         <v>21</v>
       </c>
       <c r="D115" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>80</v>
@@ -5664,7 +6283,7 @@
       <c r="L115" s="2"/>
       <c r="M115" s="2"/>
     </row>
-    <row r="116" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A116" s="2" t="s">
         <v>26</v>
       </c>
@@ -5675,7 +6294,7 @@
         <v>21</v>
       </c>
       <c r="D116" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>80</v>
@@ -5697,7 +6316,7 @@
       <c r="L116" s="2"/>
       <c r="M116" s="2"/>
     </row>
-    <row r="117" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A117" s="2" t="s">
         <v>26</v>
       </c>
@@ -5708,7 +6327,7 @@
         <v>21</v>
       </c>
       <c r="D117" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>275</v>
@@ -5730,7 +6349,7 @@
       <c r="L117" s="2"/>
       <c r="M117" s="2"/>
     </row>
-    <row r="118" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A118" s="2" t="s">
         <v>26</v>
       </c>
@@ -5741,7 +6360,7 @@
         <v>21</v>
       </c>
       <c r="D118" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>80</v>
@@ -5763,7 +6382,7 @@
       <c r="L118" s="2"/>
       <c r="M118" s="2"/>
     </row>
-    <row r="119" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A119" s="2" t="s">
         <v>26</v>
       </c>
@@ -5774,7 +6393,7 @@
         <v>21</v>
       </c>
       <c r="D119" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>80</v>
@@ -5796,7 +6415,7 @@
       <c r="L119" s="2"/>
       <c r="M119" s="2"/>
     </row>
-    <row r="120" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A120" s="2" t="s">
         <v>26</v>
       </c>
@@ -5807,7 +6426,7 @@
         <v>21</v>
       </c>
       <c r="D120" s="44" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>80</v>
@@ -5829,7 +6448,7 @@
       <c r="L120" s="2"/>
       <c r="M120" s="2"/>
     </row>
-    <row r="121" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A121" s="2" t="s">
         <v>26</v>
       </c>
@@ -5840,7 +6459,7 @@
         <v>21</v>
       </c>
       <c r="D121" s="44" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>80</v>
@@ -5862,7 +6481,7 @@
       <c r="L121" s="2"/>
       <c r="M121" s="2"/>
     </row>
-    <row r="122" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A122" s="2" t="s">
         <v>26</v>
       </c>
@@ -5873,7 +6492,7 @@
         <v>21</v>
       </c>
       <c r="D122" s="44" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>80</v>
@@ -5895,7 +6514,7 @@
       <c r="L122" s="2"/>
       <c r="M122" s="2"/>
     </row>
-    <row r="123" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A123" s="2" t="s">
         <v>26</v>
       </c>
@@ -5906,7 +6525,7 @@
         <v>21</v>
       </c>
       <c r="D123" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>30</v>
@@ -5928,7 +6547,7 @@
       <c r="L123" s="2"/>
       <c r="M123" s="2"/>
     </row>
-    <row r="124" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A124" s="2" t="s">
         <v>26</v>
       </c>
@@ -5939,7 +6558,7 @@
         <v>21</v>
       </c>
       <c r="D124" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>290</v>
@@ -5961,7 +6580,7 @@
       <c r="L124" s="2"/>
       <c r="M124" s="2"/>
     </row>
-    <row r="125" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A125" s="2" t="s">
         <v>26</v>
       </c>
@@ -5972,7 +6591,7 @@
         <v>21</v>
       </c>
       <c r="D125" s="44" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>30</v>
@@ -5994,7 +6613,7 @@
       <c r="L125" s="2"/>
       <c r="M125" s="2"/>
     </row>
-    <row r="126" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A126" s="2" t="s">
         <v>26</v>
       </c>
@@ -6005,7 +6624,7 @@
         <v>21</v>
       </c>
       <c r="D126" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>295</v>
@@ -6027,7 +6646,7 @@
       <c r="L126" s="2"/>
       <c r="M126" s="2"/>
     </row>
-    <row r="127" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A127" s="15" t="s">
         <v>26</v>
       </c>
@@ -6038,7 +6657,7 @@
         <v>21</v>
       </c>
       <c r="D127" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>275</v>
@@ -6060,7 +6679,7 @@
       <c r="L127" s="2"/>
       <c r="M127" s="2"/>
     </row>
-    <row r="128" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A128" s="2" t="s">
         <v>26</v>
       </c>
@@ -6071,7 +6690,7 @@
         <v>21</v>
       </c>
       <c r="D128" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>70</v>
@@ -6093,7 +6712,7 @@
       <c r="L128" s="2"/>
       <c r="M128" s="2"/>
     </row>
-    <row r="129" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A129" s="2" t="s">
         <v>26</v>
       </c>
@@ -6104,7 +6723,7 @@
         <v>21</v>
       </c>
       <c r="D129" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>70</v>
@@ -6126,7 +6745,7 @@
       <c r="L129" s="2"/>
       <c r="M129" s="2"/>
     </row>
-    <row r="130" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A130" s="2" t="s">
         <v>26</v>
       </c>
@@ -6137,7 +6756,7 @@
         <v>21</v>
       </c>
       <c r="D130" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>70</v>
@@ -6159,7 +6778,7 @@
       <c r="L130" s="2"/>
       <c r="M130" s="2"/>
     </row>
-    <row r="131" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A131" s="2" t="s">
         <v>26</v>
       </c>
@@ -6170,7 +6789,7 @@
         <v>21</v>
       </c>
       <c r="D131" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>70</v>
@@ -6203,7 +6822,7 @@
         <v>21</v>
       </c>
       <c r="D132" s="44" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>70</v>
@@ -6225,7 +6844,7 @@
       <c r="L132" s="2"/>
       <c r="M132" s="2"/>
     </row>
-    <row r="133" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A133" s="15" t="s">
         <v>26</v>
       </c>
@@ -6236,7 +6855,7 @@
         <v>21</v>
       </c>
       <c r="D133" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>118</v>
@@ -6258,7 +6877,7 @@
       <c r="L133" s="2"/>
       <c r="M133" s="2"/>
     </row>
-    <row r="134" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A134" s="2" t="s">
         <v>26</v>
       </c>
@@ -6269,7 +6888,7 @@
         <v>21</v>
       </c>
       <c r="D134" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>118</v>
@@ -6291,7 +6910,7 @@
       <c r="L134" s="2"/>
       <c r="M134" s="2"/>
     </row>
-    <row r="135" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A135" s="2" t="s">
         <v>26</v>
       </c>
@@ -6302,7 +6921,7 @@
         <v>21</v>
       </c>
       <c r="D135" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>123</v>
@@ -6324,7 +6943,7 @@
       <c r="L135" s="2"/>
       <c r="M135" s="2"/>
     </row>
-    <row r="136" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A136" s="2" t="s">
         <v>26</v>
       </c>
@@ -6335,7 +6954,7 @@
         <v>21</v>
       </c>
       <c r="D136" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>313</v>
@@ -6357,7 +6976,7 @@
       <c r="L136" s="2"/>
       <c r="M136" s="2"/>
     </row>
-    <row r="137" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A137" s="2" t="s">
         <v>26</v>
       </c>
@@ -6368,7 +6987,7 @@
         <v>21</v>
       </c>
       <c r="D137" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>134</v>
@@ -6390,7 +7009,7 @@
       <c r="L137" s="2"/>
       <c r="M137" s="2"/>
     </row>
-    <row r="138" spans="1:13" ht="14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:13" ht="14" x14ac:dyDescent="0.15">
       <c r="A138" s="2" t="s">
         <v>26</v>
       </c>
@@ -6401,7 +7020,7 @@
         <v>21</v>
       </c>
       <c r="D138" s="46" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>143</v>
@@ -6423,7 +7042,7 @@
       <c r="L138" s="2"/>
       <c r="M138" s="2"/>
     </row>
-    <row r="139" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A139" s="2" t="s">
         <v>26</v>
       </c>
@@ -6434,7 +7053,7 @@
         <v>21</v>
       </c>
       <c r="D139" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>134</v>
@@ -6456,7 +7075,7 @@
       <c r="L139" s="2"/>
       <c r="M139" s="2"/>
     </row>
-    <row r="140" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A140" s="2" t="s">
         <v>26</v>
       </c>
@@ -6467,7 +7086,7 @@
         <v>21</v>
       </c>
       <c r="D140" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>182</v>
@@ -6489,7 +7108,7 @@
       <c r="L140" s="2"/>
       <c r="M140" s="2"/>
     </row>
-    <row r="141" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A141" s="2" t="s">
         <v>26</v>
       </c>
@@ -6500,7 +7119,7 @@
         <v>21</v>
       </c>
       <c r="D141" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>204</v>
@@ -6522,7 +7141,7 @@
       <c r="L141" s="2"/>
       <c r="M141" s="2"/>
     </row>
-    <row r="142" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A142" s="2" t="s">
         <v>26</v>
       </c>
@@ -6533,7 +7152,7 @@
         <v>21</v>
       </c>
       <c r="D142" s="44" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>204</v>
@@ -6555,7 +7174,7 @@
       <c r="L142" s="2"/>
       <c r="M142" s="2"/>
     </row>
-    <row r="143" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A143" s="2" t="s">
         <v>26</v>
       </c>
@@ -6566,7 +7185,7 @@
         <v>21</v>
       </c>
       <c r="D143" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>187</v>
@@ -6588,7 +7207,7 @@
       <c r="L143" s="2"/>
       <c r="M143" s="2"/>
     </row>
-    <row r="144" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A144" s="2" t="s">
         <v>26</v>
       </c>
@@ -6599,7 +7218,7 @@
         <v>21</v>
       </c>
       <c r="D144" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>327</v>
@@ -6621,7 +7240,7 @@
       <c r="L144" s="2"/>
       <c r="M144" s="2"/>
     </row>
-    <row r="145" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A145" s="2" t="s">
         <v>26</v>
       </c>
@@ -6632,7 +7251,7 @@
         <v>21</v>
       </c>
       <c r="D145" s="44" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>327</v>
@@ -6654,7 +7273,7 @@
       <c r="L145" s="2"/>
       <c r="M145" s="2"/>
     </row>
-    <row r="146" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A146" s="2" t="s">
         <v>26</v>
       </c>
@@ -6665,7 +7284,7 @@
         <v>21</v>
       </c>
       <c r="D146" s="44" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>327</v>
@@ -6687,7 +7306,7 @@
       <c r="L146" s="2"/>
       <c r="M146" s="2"/>
     </row>
-    <row r="147" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A147" s="2" t="s">
         <v>26</v>
       </c>
@@ -6698,7 +7317,7 @@
         <v>21</v>
       </c>
       <c r="D147" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>222</v>
@@ -6720,7 +7339,7 @@
       <c r="L147" s="2"/>
       <c r="M147" s="2"/>
     </row>
-    <row r="148" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A148" s="2" t="s">
         <v>26</v>
       </c>
@@ -6731,7 +7350,7 @@
         <v>21</v>
       </c>
       <c r="D148" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>222</v>
@@ -6772,7 +7391,7 @@
       <c r="F149" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G149" s="2" t="s">
+      <c r="G149" s="50" t="s">
         <v>335</v>
       </c>
       <c r="H149" s="2" t="s">
@@ -6786,7 +7405,7 @@
       <c r="L149" s="2"/>
       <c r="M149" s="2"/>
     </row>
-    <row r="150" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A150" s="2" t="s">
         <v>26</v>
       </c>
@@ -6797,7 +7416,7 @@
         <v>21</v>
       </c>
       <c r="D150" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>337</v>
@@ -6819,7 +7438,7 @@
       <c r="L150" s="2"/>
       <c r="M150" s="2"/>
     </row>
-    <row r="151" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A151" s="2" t="s">
         <v>26</v>
       </c>
@@ -6830,7 +7449,7 @@
         <v>21</v>
       </c>
       <c r="D151" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>337</v>
@@ -6871,7 +7490,7 @@
       <c r="F152" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G152" s="2" t="s">
+      <c r="G152" s="50" t="s">
         <v>340</v>
       </c>
       <c r="H152" s="2" t="s">
@@ -6904,7 +7523,7 @@
       <c r="F153" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G153" s="2" t="s">
+      <c r="G153" s="50" t="s">
         <v>342</v>
       </c>
       <c r="H153" s="2" t="s">
@@ -6918,7 +7537,7 @@
       <c r="L153" s="2"/>
       <c r="M153" s="2"/>
     </row>
-    <row r="154" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A154" s="2" t="s">
         <v>26</v>
       </c>
@@ -6929,7 +7548,7 @@
         <v>21</v>
       </c>
       <c r="D154" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E154" s="2" t="s">
         <v>337</v>
@@ -6951,7 +7570,7 @@
       <c r="L154" s="2"/>
       <c r="M154" s="2"/>
     </row>
-    <row r="155" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A155" s="15" t="s">
         <v>26</v>
       </c>
@@ -6995,19 +7614,19 @@
         <v>21</v>
       </c>
       <c r="D156" s="44" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>347</v>
+        <v>406</v>
       </c>
       <c r="F156" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G156" s="49" t="s">
-        <v>407</v>
+      <c r="G156" s="53" t="s">
+        <v>401</v>
       </c>
       <c r="H156" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I156" s="15" t="s">
         <v>34</v>
@@ -7017,7 +7636,7 @@
       <c r="L156" s="2"/>
       <c r="M156" s="2"/>
     </row>
-    <row r="157" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A157" s="2" t="s">
         <v>26</v>
       </c>
@@ -7028,19 +7647,19 @@
         <v>21</v>
       </c>
       <c r="D157" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F157" s="2" t="s">
         <v>44</v>
       </c>
       <c r="G157" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="H157" s="2" t="s">
         <v>350</v>
-      </c>
-      <c r="H157" s="2" t="s">
-        <v>351</v>
       </c>
       <c r="I157" s="15" t="s">
         <v>34</v>
@@ -7050,7 +7669,7 @@
       <c r="L157" s="2"/>
       <c r="M157" s="2"/>
     </row>
-    <row r="158" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A158" s="2" t="s">
         <v>26</v>
       </c>
@@ -7064,16 +7683,16 @@
         <v>29</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F158" s="2" t="s">
         <v>44</v>
       </c>
       <c r="G158" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="H158" s="2" t="s">
         <v>353</v>
-      </c>
-      <c r="H158" s="2" t="s">
-        <v>354</v>
       </c>
       <c r="I158" s="2"/>
       <c r="J158" s="2"/>
@@ -7081,7 +7700,7 @@
       <c r="L158" s="2"/>
       <c r="M158" s="2"/>
     </row>
-    <row r="159" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A159" s="2" t="s">
         <v>51</v>
       </c>
@@ -7089,46 +7708,46 @@
         <v>20240320</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F159" s="2" t="s">
         <v>52</v>
       </c>
       <c r="G159" s="2" t="s">
-        <v>357</v>
+        <v>411</v>
       </c>
       <c r="H159" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="I159" s="2"/>
     </row>
     <row r="160" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A160" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B160" s="2">
         <v>20240320</v>
       </c>
       <c r="C160" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="E160" s="2" t="s">
         <v>360</v>
-      </c>
-      <c r="D160" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="E160" s="2" t="s">
-        <v>362</v>
       </c>
       <c r="F160" s="2" t="s">
         <v>52</v>
       </c>
       <c r="G160" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="H160" s="2"/>
       <c r="I160" s="2"/>
@@ -7141,24 +7760,24 @@
         <v>20240320</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>83</v>
       </c>
       <c r="E161" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="F161" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="G161" s="2" t="s">
         <v>364</v>
-      </c>
-      <c r="F161" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="G161" s="2" t="s">
-        <v>366</v>
       </c>
       <c r="H161" s="2"/>
       <c r="I161" s="2"/>
     </row>
-    <row r="162" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A162" s="15" t="s">
         <v>26</v>
       </c>
@@ -7169,23 +7788,23 @@
         <v>21</v>
       </c>
       <c r="D162" s="44" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="E162" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F162" s="2" t="s">
         <v>44</v>
       </c>
       <c r="G162" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H162" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="I162" s="2"/>
     </row>
-    <row r="163" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A163" s="2" t="s">
         <v>26</v>
       </c>
@@ -7199,20 +7818,20 @@
         <v>29</v>
       </c>
       <c r="E163" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F163" s="2" t="s">
         <v>44</v>
       </c>
       <c r="G163" s="38" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="H163" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="I163" s="2"/>
     </row>
-    <row r="164" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:13" ht="14" x14ac:dyDescent="0.15">
       <c r="A164" s="2" t="s">
         <v>26</v>
       </c>
@@ -7225,44 +7844,44 @@
       <c r="D164" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E164" s="2" t="s">
-        <v>372</v>
+      <c r="E164" s="49" t="s">
+        <v>409</v>
       </c>
       <c r="F164" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G164" s="2" t="s">
-        <v>373</v>
+      <c r="G164" s="51" t="s">
+        <v>410</v>
       </c>
       <c r="H164" s="2" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="165" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" ht="14" x14ac:dyDescent="0.15">
       <c r="A165" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B165" s="2">
         <v>20240320</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>83</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>375</v>
+        <v>407</v>
       </c>
       <c r="F165" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G165" s="2" t="s">
-        <v>376</v>
+      <c r="G165" s="52" t="s">
+        <v>408</v>
       </c>
       <c r="H165" s="2"/>
     </row>
-    <row r="166" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A166" s="2" t="s">
         <v>51</v>
       </c>
@@ -7270,23 +7889,23 @@
         <v>20240320</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D166" s="44" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="F166" s="2" t="s">
         <v>52</v>
       </c>
       <c r="G166" s="2" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="H166" s="2"/>
     </row>
-    <row r="167" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A167" s="15" t="s">
         <v>26</v>
       </c>
@@ -7297,7 +7916,7 @@
         <v>21</v>
       </c>
       <c r="D167" s="44" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="E167" s="2" t="s">
         <v>187</v>
@@ -7306,13 +7925,13 @@
         <v>28</v>
       </c>
       <c r="G167" s="2" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="H167" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="168" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A168" s="2" t="s">
         <v>26</v>
       </c>
@@ -7323,19 +7942,19 @@
         <v>21</v>
       </c>
       <c r="D168" s="44" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="E168" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F168" s="2" t="s">
         <v>44</v>
       </c>
       <c r="G168" s="2" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="H168" s="2" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
     </row>
     <row r="169" spans="1:13" ht="13" x14ac:dyDescent="0.15">
@@ -7346,22 +7965,22 @@
         <v>20240319</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>83</v>
       </c>
       <c r="E169" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F169" s="2" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="G169" s="42" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="H169" s="2" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="170" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
@@ -7378,16 +7997,16 @@
         <v>83</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="F170" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G170" s="2" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="H170" s="2" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="I170" s="2"/>
       <c r="M170" s="2"/>
@@ -7404,24 +8023,24 @@
       </c>
       <c r="D171" s="2"/>
       <c r="E171" s="2" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="F171" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G171" s="2" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="H171" s="2" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="I171" s="2" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
     </row>
     <row r="172" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A172" s="2" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="B172" s="2">
         <v>20240602</v>
@@ -7433,18 +8052,18 @@
         <v>83</v>
       </c>
       <c r="E172" s="2" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="F172" s="2" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="G172" s="2" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
     </row>
     <row r="173" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A173" s="2" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="B173" s="2">
         <v>20240602</v>
@@ -7456,42 +8075,42 @@
         <v>29</v>
       </c>
       <c r="E173" s="2" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="F173" s="2" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="G173" s="2" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="H173" s="2" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
     </row>
     <row r="176" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G176" s="48" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
     </row>
     <row r="177" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G177" s="48" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
     </row>
     <row r="178" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G178" s="48" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
     </row>
     <row r="179" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F179" s="47"/>
       <c r="G179" s="48" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
     </row>
     <row r="180" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G180" s="48" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="193" spans="1:8" ht="13" x14ac:dyDescent="0.15">
@@ -7541,11 +8160,6 @@
         <filter val="_x0008_IOS"/>
         <filter val="iOS, 안드로이드"/>
         <filter val="iOS, Android"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="3">
-      <filters>
-        <filter val="_x0008_상"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
refactoring - postedVC 디자인패턴 변환                     MVVM 전환, UI 분리 중
</commit_message>
<xml_diff>
--- a/복사본 STUDYHUB QA.xlsx
+++ b/복사본 STUDYHUB QA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yong/Desktop/study-hub-iOS-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15C93DE-3508-8A43-94EB-CE18D0680AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4181438E-29B1-F842-B5A0-02D8BA5D7697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
@@ -3193,8 +3193,8 @@
   </sheetPr>
   <dimension ref="A1:P196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D145" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G159" sqref="G159"/>
+    <sheetView tabSelected="1" topLeftCell="C117" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G167" sqref="G167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5708,7 +5708,7 @@
       <c r="F98" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G98" s="2" t="s">
+      <c r="G98" s="50" t="s">
         <v>228</v>
       </c>
       <c r="H98" s="2" t="s">

</xml_diff>